<commit_message>
commit TPO 14 section 2
</commit_message>
<xml_diff>
--- a/Listening/Questions.xlsx
+++ b/Listening/Questions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="364">
   <si>
     <t>TPO 11</t>
   </si>
@@ -110,6 +110,15 @@
   </si>
   <si>
     <t>microClimate（Biology）</t>
+  </si>
+  <si>
+    <t>Prepare for a career in Journalism</t>
+  </si>
+  <si>
+    <t>Seafarers and Stars(Astronomy)</t>
+  </si>
+  <si>
+    <t>Passage Graves(archeology)</t>
   </si>
   <si>
     <t>Basic Comprehension Question</t>
@@ -372,6 +381,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>2+</t>
     </r>
     <r>
@@ -383,6 +398,22 @@
       </rPr>
       <t>1
 对于书架没人整理、有人quit的部分完全没听见</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>2+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>1
+出现错误的和没听到的（实际出现的）一定不能选错误的
+后文提到，ones that students and professors here would want to read about等价于inform students and faculty of an issue</t>
     </r>
   </si>
   <si>
@@ -500,6 +531,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>1+</t>
     </r>
     <r>
@@ -619,6 +656,9 @@
 正确选项是因为：Of course with reptiles, it’s a balancing act</t>
   </si>
   <si>
+    <t>1 I barely recognize couples of paragraphs表明被改了很多。上文别夸出色，这里其实想说不是他的功劳，而不是惊讶</t>
+  </si>
+  <si>
     <t>Raw Points</t>
   </si>
   <si>
@@ -694,6 +734,21 @@
     <t>喘气</t>
   </si>
   <si>
+    <t>it’s been a while since we touched base.</t>
+  </si>
+  <si>
+    <t>距离我们开始已经有段时间了</t>
+  </si>
+  <si>
+    <t>seafarer</t>
+  </si>
+  <si>
+    <t>船员</t>
+  </si>
+  <si>
+    <t>archeology听成了architecture，不可饶恕！</t>
+  </si>
+  <si>
     <t>that's odd</t>
   </si>
   <si>
@@ -760,6 +815,32 @@
     <t>躲到凉快的地方</t>
   </si>
   <si>
+    <t>byline</t>
+  </si>
+  <si>
+    <t>署名</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">navigational </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.25"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>aids</t>
+    </r>
+  </si>
+  <si>
+    <t>Isle</t>
+  </si>
+  <si>
+    <t>岛</t>
+  </si>
+  <si>
     <t>payroll</t>
   </si>
   <si>
@@ -829,6 +910,21 @@
     <t>地洞</t>
   </si>
   <si>
+    <t>hooked</t>
+  </si>
+  <si>
+    <t>入迷了</t>
+  </si>
+  <si>
+    <t>Viking</t>
+  </si>
+  <si>
+    <t>北欧海盗</t>
+  </si>
+  <si>
+    <t>which don’t get me wrong is remarkable enough</t>
+  </si>
+  <si>
     <t>retrieved</t>
   </si>
   <si>
@@ -921,6 +1017,41 @@
     <t>大量的</t>
   </si>
   <si>
+    <t>Sounds like you’ve got a real knack for this.</t>
+  </si>
+  <si>
+    <t>听起来你找到了突破口</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Long before the development of ummm </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>advanced</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> navigational tools...</t>
+    </r>
+  </si>
+  <si>
+    <t>bronze</t>
+  </si>
+  <si>
+    <t>青铜</t>
+  </si>
+  <si>
     <t>a month behind the bill</t>
   </si>
   <si>
@@ -1053,6 +1184,24 @@
     <t>外出觅食</t>
   </si>
   <si>
+    <t>Supreme Court</t>
+  </si>
+  <si>
+    <t>高级法院</t>
+  </si>
+  <si>
+    <t>islander</t>
+  </si>
+  <si>
+    <t>岛上居民</t>
+  </si>
+  <si>
+    <t>tombs</t>
+  </si>
+  <si>
+    <t>坟墓</t>
+  </si>
+  <si>
     <t>my tuitions due soon</t>
   </si>
   <si>
@@ -1140,6 +1289,12 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
       <t>But the ease wi</t>
     </r>
     <r>
@@ -1165,6 +1320,24 @@
     <t>out foraging for food</t>
   </si>
   <si>
+    <t>pre-law class</t>
+  </si>
+  <si>
+    <t>法律预备课程</t>
+  </si>
+  <si>
+    <t>partition</t>
+  </si>
+  <si>
+    <t>划分</t>
+  </si>
+  <si>
+    <t>enclose</t>
+  </si>
+  <si>
+    <t>裹在内部</t>
+  </si>
+  <si>
     <t>count on it</t>
   </si>
   <si>
@@ -1239,6 +1412,34 @@
     <t>流汗</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">much more </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">symmetrically </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>than it could farther away the equator</t>
+    </r>
+  </si>
+  <si>
+    <t>overlapping</t>
+  </si>
+  <si>
+    <t>叠在一起的</t>
+  </si>
+  <si>
     <t>secularization</t>
   </si>
   <si>
@@ -1319,6 +1520,76 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve">it was easier to </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>discern the order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> in the sky </t>
+    </r>
+  </si>
+  <si>
+    <t>识别</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">with chambers that were flooded with sunlight on certain special days of the year, which must have seemed </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">miraculous </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">and inspired a good deal of </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve">religious </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>wonder</t>
+    </r>
+  </si>
+  <si>
+    <t>不可思议的</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
@@ -1366,6 +1637,35 @@
   </si>
   <si>
     <r>
+      <t xml:space="preserve"> And they realized that you had to know the stars </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>in order to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> navigate</t>
+    </r>
+  </si>
+  <si>
+    <t>chanting</t>
+  </si>
+  <si>
+    <t>念经</t>
+  </si>
+  <si>
+    <r>
       <rPr>
         <b/>
         <sz val="11"/>
@@ -1426,6 +1726,35 @@
     <t>流星</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">When you </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.35"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>wanted</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> a star expert, you asked for a navigator.</t>
+    </r>
+  </si>
+  <si>
+    <t>bouncing off</t>
+  </si>
+  <si>
+    <t>碰撞</t>
+  </si>
+  <si>
     <t>clergy</t>
   </si>
   <si>
@@ -1444,6 +1773,18 @@
     <t>陨星</t>
   </si>
   <si>
+    <t>constellations</t>
+  </si>
+  <si>
+    <t>星座</t>
+  </si>
+  <si>
+    <t>intriguing</t>
+  </si>
+  <si>
+    <t>令人费解的</t>
+  </si>
+  <si>
     <t>vernacular</t>
   </si>
   <si>
@@ -1453,6 +1794,18 @@
     <t>He’s very conscious of</t>
   </si>
   <si>
+    <t>directly</t>
+  </si>
+  <si>
+    <t>dgrectly</t>
+  </si>
+  <si>
+    <t>standing waves</t>
+  </si>
+  <si>
+    <t>驻波</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1488,6 +1841,12 @@
     <t>某种程度上</t>
   </si>
   <si>
+    <t>deafening</t>
+  </si>
+  <si>
+    <t>震耳欲聋</t>
+  </si>
+  <si>
     <t>satire</t>
   </si>
   <si>
@@ -1523,6 +1882,12 @@
     </r>
   </si>
   <si>
+    <t>acoustics</t>
+  </si>
+  <si>
+    <t>音响效果</t>
+  </si>
+  <si>
     <t>imprisonment</t>
   </si>
   <si>
@@ -1535,6 +1900,12 @@
     <t>虚构的</t>
   </si>
   <si>
+    <t>engender</t>
+  </si>
+  <si>
+    <t>产生</t>
+  </si>
+  <si>
     <t>persecution</t>
   </si>
   <si>
@@ -1547,6 +1918,12 @@
     <t>拼凑</t>
   </si>
   <si>
+    <t>awe</t>
+  </si>
+  <si>
+    <t>敬畏</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="11"/>
@@ -1589,40 +1966,119 @@
     <t>冒着被监禁或被迫害的风险去写作。</t>
   </si>
   <si>
+    <t>worshiper</t>
+  </si>
+  <si>
+    <t>礼拜者</t>
+  </si>
+  <si>
     <t>resurrected</t>
   </si>
   <si>
     <t>复兴的</t>
   </si>
   <si>
+    <t>resonance</t>
+  </si>
+  <si>
+    <t>共振</t>
+  </si>
+  <si>
     <t>not to say</t>
   </si>
   <si>
     <t>甚至是</t>
   </si>
   <si>
+    <t>ring out</t>
+  </si>
+  <si>
+    <t>发出</t>
+  </si>
+  <si>
     <t>melodramatic</t>
   </si>
   <si>
     <t>情节性的</t>
   </si>
   <si>
+    <r>
+      <t xml:space="preserve">we’re mysteriously </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>agitated</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> by it</t>
+    </r>
+  </si>
+  <si>
+    <t>感到烦躁</t>
+  </si>
+  <si>
     <t>confined</t>
   </si>
   <si>
     <t>局限于</t>
   </si>
   <si>
+    <t>dizziness</t>
+  </si>
+  <si>
+    <t>眩晕</t>
+  </si>
+  <si>
     <t>any more than</t>
   </si>
   <si>
     <t>不至于</t>
   </si>
   <si>
+    <t>that sort of thing you see</t>
+  </si>
+  <si>
     <t>major divide</t>
   </si>
   <si>
     <t>格局划分</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">certainly </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t>with regard to</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="微软雅黑"/>
+        <charset val="134"/>
+      </rPr>
+      <t xml:space="preserve"> astronomical or calendar function that seems pretty obvious</t>
+    </r>
+  </si>
+  <si>
+    <t>不必赘述</t>
   </si>
   <si>
     <t>cadence</t>
@@ -1727,7 +2183,7 @@
     <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="26">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1752,6 +2208,12 @@
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1912,7 +2374,19 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0" tint="-0.25"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFFC000"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.35"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
@@ -2246,10 +2720,10 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2258,34 +2732,31 @@
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -2297,98 +2768,101 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -2439,6 +2913,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -2790,8 +3270,8 @@
   <sheetPr/>
   <dimension ref="A1:AQ46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="AJ13" sqref="AJ13"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="AO36" sqref="AO36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15.6"/>
@@ -2825,13 +3305,19 @@
     <col min="27" max="27" width="26.5092592592593" style="1" hidden="1" customWidth="1"/>
     <col min="28" max="28" width="19.8333333333333" style="1" hidden="1" customWidth="1"/>
     <col min="29" max="29" width="19.6851851851852" style="1" hidden="1" customWidth="1"/>
-    <col min="30" max="30" width="22.537037037037" style="4" customWidth="1"/>
-    <col min="31" max="31" width="15.8703703703704" style="4" customWidth="1"/>
-    <col min="32" max="32" width="26.5" style="4" customWidth="1"/>
-    <col min="33" max="33" width="20.787037037037" style="4" customWidth="1"/>
+    <col min="30" max="30" width="22.537037037037" style="1" customWidth="1"/>
+    <col min="31" max="31" width="15.8703703703704" style="1" customWidth="1"/>
+    <col min="32" max="32" width="26.5" style="1" customWidth="1"/>
+    <col min="33" max="33" width="20.787037037037" style="1" customWidth="1"/>
     <col min="34" max="34" width="31.4259259259259" style="2" customWidth="1"/>
     <col min="35" max="35" width="21.2685185185185" style="2" customWidth="1"/>
-    <col min="36" max="16384" width="9" style="2"/>
+    <col min="36" max="36" width="16.037037037037" style="4" customWidth="1"/>
+    <col min="37" max="37" width="19.0462962962963" style="4" customWidth="1"/>
+    <col min="38" max="38" width="14.1203703703704" style="4" customWidth="1"/>
+    <col min="39" max="39" width="16.1944444444444" style="4" customWidth="1"/>
+    <col min="40" max="40" width="21.5833333333333" style="4" customWidth="1"/>
+    <col min="41" max="41" width="10.4722222222222" style="4" customWidth="1"/>
+    <col min="42" max="16384" width="9" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41">
@@ -2878,12 +3364,12 @@
       <c r="AG1" s="12"/>
       <c r="AH1" s="11"/>
       <c r="AI1" s="11"/>
-      <c r="AJ1" s="11"/>
-      <c r="AK1" s="11"/>
-      <c r="AL1" s="11"/>
-      <c r="AM1" s="11"/>
-      <c r="AN1" s="11"/>
-      <c r="AO1" s="11"/>
+      <c r="AJ1" s="12"/>
+      <c r="AK1" s="12"/>
+      <c r="AL1" s="12"/>
+      <c r="AM1" s="12"/>
+      <c r="AN1" s="12"/>
+      <c r="AO1" s="12"/>
     </row>
     <row r="2" s="1" customFormat="1" ht="31.2" spans="1:41">
       <c r="A2" s="7"/>
@@ -2963,19 +3449,25 @@
         <v>24</v>
       </c>
       <c r="AI2" s="12"/>
-      <c r="AJ2" s="12"/>
+      <c r="AJ2" s="12" t="s">
+        <v>25</v>
+      </c>
       <c r="AK2" s="12"/>
-      <c r="AL2" s="12"/>
+      <c r="AL2" s="12" t="s">
+        <v>26</v>
+      </c>
       <c r="AM2" s="12"/>
-      <c r="AN2" s="12"/>
+      <c r="AN2" s="12" t="s">
+        <v>27</v>
+      </c>
       <c r="AO2" s="12"/>
     </row>
     <row r="3" ht="59" customHeight="1" spans="1:41">
       <c r="A3" s="9" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6">
@@ -2993,7 +3485,7 @@
       </c>
       <c r="I3" s="5"/>
       <c r="J3" s="13" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="K3" s="5">
         <v>1</v>
@@ -3001,7 +3493,7 @@
       <c r="L3" s="12"/>
       <c r="M3" s="12"/>
       <c r="N3" s="14" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O3" s="12"/>
       <c r="P3" s="11">
@@ -3040,17 +3532,23 @@
         <v>1</v>
       </c>
       <c r="AI3" s="11"/>
-      <c r="AJ3" s="11"/>
-      <c r="AK3" s="11"/>
-      <c r="AL3" s="11"/>
-      <c r="AM3" s="11"/>
-      <c r="AN3" s="11"/>
-      <c r="AO3" s="11"/>
+      <c r="AJ3" s="12">
+        <v>1</v>
+      </c>
+      <c r="AK3" s="12"/>
+      <c r="AL3" s="12">
+        <v>1</v>
+      </c>
+      <c r="AM3" s="12"/>
+      <c r="AN3" s="12">
+        <v>1</v>
+      </c>
+      <c r="AO3" s="12"/>
     </row>
     <row r="4" ht="33" customHeight="1" spans="1:43">
       <c r="A4" s="9"/>
       <c r="B4" s="7" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="C4" s="6">
         <v>1</v>
@@ -3097,32 +3595,32 @@
       <c r="AG4" s="12"/>
       <c r="AH4" s="11"/>
       <c r="AI4" s="11"/>
-      <c r="AJ4" s="11"/>
-      <c r="AK4" s="11"/>
-      <c r="AL4" s="11"/>
-      <c r="AM4" s="11"/>
-      <c r="AN4" s="11"/>
-      <c r="AO4" s="11"/>
+      <c r="AJ4" s="12"/>
+      <c r="AK4" s="12"/>
+      <c r="AL4" s="12"/>
+      <c r="AM4" s="12"/>
+      <c r="AN4" s="12"/>
+      <c r="AO4" s="12"/>
       <c r="AP4" s="11"/>
       <c r="AQ4" s="11"/>
     </row>
     <row r="5" ht="78" spans="1:43">
       <c r="A5" s="9"/>
       <c r="B5" s="5" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="C5" s="6"/>
       <c r="D5" s="8" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F5" s="6">
         <v>1</v>
       </c>
       <c r="G5" s="10" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="H5" s="6">
         <v>1</v>
@@ -3131,7 +3629,7 @@
         <v>3</v>
       </c>
       <c r="J5" s="7" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K5" s="5">
         <v>2</v>
@@ -3141,11 +3639,11 @@
       </c>
       <c r="M5" s="12"/>
       <c r="N5" s="12" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="O5" s="12"/>
       <c r="P5" s="12" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="Q5" s="12"/>
       <c r="R5" s="12">
@@ -3161,7 +3659,7 @@
       </c>
       <c r="W5" s="12"/>
       <c r="X5" s="12" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="Y5" s="12"/>
       <c r="Z5" s="12">
@@ -3169,11 +3667,11 @@
       </c>
       <c r="AA5" s="12"/>
       <c r="AB5" s="12" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="AC5" s="12"/>
       <c r="AD5" s="12" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="AE5" s="12"/>
       <c r="AF5" s="12">
@@ -3184,21 +3682,27 @@
         <v>3</v>
       </c>
       <c r="AI5" s="11"/>
-      <c r="AJ5" s="11"/>
-      <c r="AK5" s="11"/>
-      <c r="AL5" s="11"/>
-      <c r="AM5" s="11"/>
-      <c r="AN5" s="11"/>
-      <c r="AO5" s="11"/>
+      <c r="AJ5" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="AK5" s="12"/>
+      <c r="AL5" s="12">
+        <v>3</v>
+      </c>
+      <c r="AM5" s="12"/>
+      <c r="AN5" s="12">
+        <v>2</v>
+      </c>
+      <c r="AO5" s="12"/>
       <c r="AP5" s="11"/>
       <c r="AQ5" s="11"/>
     </row>
     <row r="6" ht="78" spans="1:43">
       <c r="A6" s="9" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C6" s="6">
         <v>2</v>
@@ -3210,10 +3714,10 @@
         <v>2</v>
       </c>
       <c r="F6" s="8" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="G6" s="8" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="H6" s="6">
         <v>3</v>
@@ -3228,7 +3732,7 @@
       <c r="L6" s="12"/>
       <c r="M6" s="12"/>
       <c r="N6" s="14" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="O6" s="12"/>
       <c r="P6" s="11">
@@ -3244,7 +3748,7 @@
       </c>
       <c r="U6" s="12"/>
       <c r="V6" s="12" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="W6" s="12"/>
       <c r="X6" s="12"/>
@@ -3262,26 +3766,30 @@
       </c>
       <c r="AE6" s="12"/>
       <c r="AF6" s="12" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="AG6" s="12"/>
       <c r="AH6" s="14" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="AI6" s="11"/>
-      <c r="AJ6" s="11"/>
-      <c r="AK6" s="11"/>
-      <c r="AL6" s="11"/>
-      <c r="AM6" s="11"/>
-      <c r="AN6" s="11"/>
-      <c r="AO6" s="11"/>
+      <c r="AJ6" s="12"/>
+      <c r="AK6" s="12"/>
+      <c r="AL6" s="12">
+        <v>1</v>
+      </c>
+      <c r="AM6" s="12"/>
+      <c r="AN6" s="12">
+        <v>2</v>
+      </c>
+      <c r="AO6" s="12"/>
       <c r="AP6" s="11"/>
       <c r="AQ6" s="11"/>
     </row>
     <row r="7" ht="109.2" spans="1:43">
       <c r="A7" s="9"/>
       <c r="B7" s="7" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C7" s="6">
         <v>1</v>
@@ -3295,7 +3803,7 @@
         <v>1</v>
       </c>
       <c r="J7" s="13" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="K7" s="5"/>
       <c r="L7" s="12"/>
@@ -3319,7 +3827,7 @@
       <c r="X7" s="12"/>
       <c r="Y7" s="12"/>
       <c r="Z7" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="AA7" s="12"/>
       <c r="AB7" s="12"/>
@@ -3330,21 +3838,21 @@
       <c r="AG7" s="12"/>
       <c r="AH7" s="11"/>
       <c r="AI7" s="11"/>
-      <c r="AJ7" s="11"/>
-      <c r="AK7" s="11"/>
-      <c r="AL7" s="11"/>
-      <c r="AM7" s="11"/>
-      <c r="AN7" s="11"/>
-      <c r="AO7" s="11"/>
+      <c r="AJ7" s="12"/>
+      <c r="AK7" s="12"/>
+      <c r="AL7" s="12"/>
+      <c r="AM7" s="12"/>
+      <c r="AN7" s="12"/>
+      <c r="AO7" s="12"/>
       <c r="AP7" s="11"/>
       <c r="AQ7" s="11"/>
     </row>
     <row r="8" ht="31.2" spans="1:43">
       <c r="A8" s="9" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C8" s="6"/>
       <c r="D8" s="6"/>
@@ -3356,7 +3864,7 @@
       <c r="J8" s="5"/>
       <c r="K8" s="5"/>
       <c r="L8" s="12" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="M8" s="12"/>
       <c r="N8" s="12"/>
@@ -3381,19 +3889,19 @@
       <c r="AG8" s="12"/>
       <c r="AH8" s="11"/>
       <c r="AI8" s="11"/>
-      <c r="AJ8" s="11"/>
-      <c r="AK8" s="11"/>
-      <c r="AL8" s="11"/>
-      <c r="AM8" s="11"/>
-      <c r="AN8" s="11"/>
-      <c r="AO8" s="11"/>
+      <c r="AJ8" s="12"/>
+      <c r="AK8" s="12"/>
+      <c r="AL8" s="12"/>
+      <c r="AM8" s="12"/>
+      <c r="AN8" s="12"/>
+      <c r="AO8" s="12"/>
       <c r="AP8" s="11"/>
       <c r="AQ8" s="11"/>
     </row>
     <row r="9" ht="31.2" spans="1:43">
       <c r="A9" s="9"/>
       <c r="B9" s="7" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -3432,19 +3940,19 @@
       <c r="AG9" s="12"/>
       <c r="AH9" s="11"/>
       <c r="AI9" s="11"/>
-      <c r="AJ9" s="11"/>
-      <c r="AK9" s="11"/>
-      <c r="AL9" s="11"/>
-      <c r="AM9" s="11"/>
-      <c r="AN9" s="11"/>
-      <c r="AO9" s="11"/>
+      <c r="AJ9" s="12"/>
+      <c r="AK9" s="12"/>
+      <c r="AL9" s="12"/>
+      <c r="AM9" s="12"/>
+      <c r="AN9" s="12"/>
+      <c r="AO9" s="12"/>
       <c r="AP9" s="11"/>
       <c r="AQ9" s="11"/>
     </row>
     <row r="10" ht="75" customHeight="1" spans="1:43">
       <c r="A10" s="9"/>
       <c r="B10" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C10" s="6">
         <v>1</v>
@@ -3460,17 +3968,17 @@
       </c>
       <c r="I10" s="5"/>
       <c r="J10" s="13" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="K10" s="13" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="L10" s="12">
         <v>1</v>
       </c>
       <c r="M10" s="12"/>
       <c r="N10" s="12" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="O10" s="12"/>
       <c r="P10" s="11"/>
@@ -3496,21 +4004,27 @@
       <c r="AF10" s="12"/>
       <c r="AG10" s="12"/>
       <c r="AH10" s="14" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="AI10" s="16"/>
-      <c r="AJ10" s="11"/>
-      <c r="AK10" s="11"/>
-      <c r="AL10" s="11"/>
-      <c r="AM10" s="11"/>
-      <c r="AN10" s="11"/>
-      <c r="AO10" s="11"/>
+      <c r="AJ10" s="14" t="s">
+        <v>64</v>
+      </c>
+      <c r="AK10" s="14"/>
+      <c r="AL10" s="12">
+        <v>1</v>
+      </c>
+      <c r="AM10" s="12"/>
+      <c r="AN10" s="12">
+        <v>1</v>
+      </c>
+      <c r="AO10" s="12"/>
       <c r="AP10" s="11"/>
       <c r="AQ10" s="11"/>
     </row>
     <row r="11" spans="1:17">
       <c r="A11" s="5" t="s">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="B11" s="5"/>
       <c r="C11" s="6">
@@ -3535,7 +4049,7 @@
     </row>
     <row r="12" spans="1:17">
       <c r="A12" s="5" t="s">
-        <v>61</v>
+        <v>66</v>
       </c>
       <c r="B12" s="5"/>
       <c r="C12" s="6">
@@ -3556,7 +4070,7 @@
       <c r="P12" s="11"/>
       <c r="Q12" s="11"/>
     </row>
-    <row r="13" ht="62.4" spans="1:35">
+    <row r="13" ht="62.4" spans="1:40">
       <c r="A13" s="5"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
@@ -3566,80 +4080,95 @@
       <c r="G13" s="6"/>
       <c r="H13" s="6"/>
       <c r="I13" s="5" t="s">
-        <v>62</v>
+        <v>67</v>
       </c>
       <c r="J13" s="5" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="K13" s="5"/>
       <c r="L13" s="7" t="s">
         <v>13</v>
       </c>
       <c r="M13" s="5" t="s">
-        <v>64</v>
+        <v>69</v>
       </c>
       <c r="N13" s="7" t="s">
-        <v>65</v>
+        <v>70</v>
       </c>
       <c r="O13" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P13" s="1" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>68</v>
+        <v>73</v>
       </c>
       <c r="R13" s="1" t="s">
-        <v>69</v>
+        <v>74</v>
       </c>
       <c r="S13" s="1" t="s">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="T13" s="1" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="V13" s="1" t="s">
-        <v>72</v>
+        <v>77</v>
       </c>
       <c r="W13" s="1" t="s">
-        <v>73</v>
+        <v>78</v>
       </c>
       <c r="X13" s="1" t="s">
-        <v>74</v>
+        <v>79</v>
       </c>
       <c r="Y13" s="1" t="s">
-        <v>75</v>
+        <v>80</v>
       </c>
       <c r="Z13" s="1" t="s">
-        <v>76</v>
+        <v>81</v>
       </c>
       <c r="AA13" s="1" t="s">
-        <v>77</v>
+        <v>82</v>
       </c>
       <c r="AB13" s="1" t="s">
-        <v>78</v>
+        <v>83</v>
       </c>
       <c r="AC13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="AD13" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="AF13" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="AG13" s="4" t="s">
-        <v>82</v>
+        <v>84</v>
+      </c>
+      <c r="AD13" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="AF13" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="AG13" s="1" t="s">
+        <v>87</v>
       </c>
       <c r="AH13" s="2" t="s">
-        <v>83</v>
+        <v>88</v>
       </c>
       <c r="AI13" s="2" t="s">
-        <v>84</v>
+        <v>89</v>
+      </c>
+      <c r="AJ13" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="AK13" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="AL13" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="AM13" s="4" t="s">
+        <v>93</v>
+      </c>
+      <c r="AN13" s="17" t="s">
+        <v>94</v>
       </c>
     </row>
-    <row r="14" ht="62.4" spans="1:35">
+    <row r="14" ht="62.4" spans="1:41">
       <c r="A14" s="5"/>
       <c r="B14" s="5"/>
       <c r="C14" s="6"/>
@@ -3652,74 +4181,89 @@
       <c r="J14" s="5"/>
       <c r="K14" s="5"/>
       <c r="L14" s="7" t="s">
-        <v>85</v>
+        <v>95</v>
       </c>
       <c r="M14" s="5"/>
       <c r="N14" s="7" t="s">
-        <v>86</v>
+        <v>96</v>
       </c>
       <c r="O14" s="5" t="s">
-        <v>87</v>
+        <v>97</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>88</v>
+        <v>98</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>89</v>
+        <v>99</v>
       </c>
       <c r="R14" s="1" t="s">
-        <v>90</v>
+        <v>100</v>
       </c>
       <c r="S14" s="1" t="s">
-        <v>91</v>
+        <v>101</v>
       </c>
       <c r="T14" s="1" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
       <c r="U14" s="1" t="s">
-        <v>93</v>
+        <v>103</v>
       </c>
       <c r="V14" s="1" t="s">
-        <v>94</v>
+        <v>104</v>
       </c>
       <c r="W14" s="1" t="s">
-        <v>95</v>
+        <v>105</v>
       </c>
       <c r="X14" s="1" t="s">
-        <v>96</v>
+        <v>106</v>
       </c>
       <c r="Z14" s="1" t="s">
-        <v>97</v>
+        <v>107</v>
       </c>
       <c r="AA14" s="1" t="s">
-        <v>98</v>
+        <v>108</v>
       </c>
       <c r="AB14" s="1" t="s">
-        <v>99</v>
+        <v>109</v>
       </c>
       <c r="AC14" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="AD14" s="4" t="s">
-        <v>101</v>
-      </c>
-      <c r="AE14" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="AF14" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="AG14" s="4" t="s">
-        <v>104</v>
+        <v>110</v>
+      </c>
+      <c r="AD14" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="AE14" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="AF14" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="AG14" s="1" t="s">
+        <v>114</v>
       </c>
       <c r="AH14" s="2" t="s">
-        <v>105</v>
+        <v>115</v>
       </c>
       <c r="AI14" s="2" t="s">
-        <v>106</v>
+        <v>116</v>
+      </c>
+      <c r="AJ14" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="AK14" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="AL14" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="AN14" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="AO14" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
-    <row r="15" ht="31.2" spans="1:35">
+    <row r="15" ht="62.4" spans="1:40">
       <c r="A15" s="5"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
@@ -3732,79 +4276,94 @@
       <c r="J15" s="5"/>
       <c r="K15" s="5"/>
       <c r="L15" s="7" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="M15" s="5" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="N15" s="7" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="O15" s="5" t="s">
-        <v>66</v>
+        <v>71</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="R15" s="1" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="S15" s="1" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="T15" s="1" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="U15" s="1" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="V15" s="1" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="W15" s="1" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="X15" s="1" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="Y15" s="1" t="s">
-        <v>119</v>
+        <v>134</v>
       </c>
       <c r="Z15" s="1" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="AA15" s="1" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="AB15" s="1" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="AC15" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="AD15" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="AE15" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="AF15" s="4" t="s">
-        <v>126</v>
-      </c>
-      <c r="AG15" s="4" t="s">
-        <v>127</v>
+        <v>138</v>
+      </c>
+      <c r="AD15" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AE15" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AF15" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AG15" s="1" t="s">
+        <v>142</v>
       </c>
       <c r="AH15" s="2" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="AI15" s="2" t="s">
-        <v>129</v>
+        <v>144</v>
+      </c>
+      <c r="AJ15" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="AK15" s="4" t="s">
+        <v>146</v>
+      </c>
+      <c r="AL15" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="AM15" s="4" t="s">
+        <v>148</v>
+      </c>
+      <c r="AN15" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
-    <row r="16" ht="46.8" spans="1:35">
+    <row r="16" ht="109.2" spans="1:41">
       <c r="A16" s="5"/>
       <c r="B16" s="5"/>
       <c r="C16" s="6"/>
@@ -3817,73 +4376,88 @@
       <c r="J16" s="5"/>
       <c r="K16" s="5"/>
       <c r="L16" s="7" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="M16" s="5" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="N16" s="7" t="s">
-        <v>132</v>
+        <v>152</v>
       </c>
       <c r="O16" s="5" t="s">
-        <v>133</v>
+        <v>153</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>134</v>
+        <v>154</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>135</v>
+        <v>155</v>
       </c>
       <c r="R16" s="1" t="s">
-        <v>136</v>
+        <v>156</v>
       </c>
       <c r="S16" s="1" t="s">
-        <v>137</v>
+        <v>157</v>
       </c>
       <c r="T16" s="1" t="s">
-        <v>138</v>
+        <v>158</v>
       </c>
       <c r="V16" s="1" t="s">
-        <v>139</v>
+        <v>159</v>
       </c>
       <c r="W16" s="1" t="s">
-        <v>140</v>
+        <v>160</v>
       </c>
       <c r="X16" s="1" t="s">
-        <v>141</v>
+        <v>161</v>
       </c>
       <c r="Y16" s="1" t="s">
-        <v>142</v>
+        <v>162</v>
       </c>
       <c r="Z16" s="1" t="s">
-        <v>143</v>
+        <v>163</v>
       </c>
       <c r="AA16" s="1" t="s">
-        <v>144</v>
+        <v>164</v>
       </c>
       <c r="AB16" s="1" t="s">
-        <v>145</v>
+        <v>165</v>
       </c>
       <c r="AC16" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="AD16" s="4" t="s">
-        <v>147</v>
-      </c>
-      <c r="AF16" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="AG16" s="4" t="s">
-        <v>149</v>
+        <v>166</v>
+      </c>
+      <c r="AD16" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="AF16" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="AG16" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="AH16" s="2" t="s">
-        <v>150</v>
+        <v>170</v>
       </c>
       <c r="AI16" s="2" t="s">
-        <v>151</v>
+        <v>171</v>
+      </c>
+      <c r="AJ16" s="4" t="s">
+        <v>172</v>
+      </c>
+      <c r="AK16" s="4" t="s">
+        <v>173</v>
+      </c>
+      <c r="AL16" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="AN16" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="AO16" s="4" t="s">
+        <v>176</v>
       </c>
     </row>
-    <row r="17" ht="78" spans="1:35">
+    <row r="17" ht="78" spans="1:41">
       <c r="A17" s="5"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
@@ -3896,62 +4470,80 @@
       <c r="J17" s="5"/>
       <c r="K17" s="5"/>
       <c r="L17" s="7" t="s">
-        <v>152</v>
+        <v>177</v>
       </c>
       <c r="M17" s="5"/>
       <c r="N17" s="7" t="s">
-        <v>153</v>
+        <v>178</v>
       </c>
       <c r="O17" s="5" t="s">
-        <v>154</v>
+        <v>179</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>155</v>
+        <v>180</v>
       </c>
       <c r="R17" s="1" t="s">
-        <v>156</v>
+        <v>181</v>
       </c>
       <c r="T17" s="1" t="s">
-        <v>157</v>
+        <v>182</v>
       </c>
       <c r="U17" s="1" t="s">
-        <v>158</v>
+        <v>183</v>
       </c>
       <c r="V17" s="1" t="s">
-        <v>159</v>
+        <v>184</v>
       </c>
       <c r="X17" s="1" t="s">
-        <v>160</v>
+        <v>185</v>
       </c>
       <c r="Z17" s="1" t="s">
-        <v>161</v>
+        <v>186</v>
       </c>
       <c r="AA17" s="1" t="s">
-        <v>162</v>
+        <v>187</v>
       </c>
       <c r="AB17" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="AD17" s="4" t="s">
-        <v>164</v>
-      </c>
-      <c r="AE17" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="AF17" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="AG17" s="4" t="s">
-        <v>167</v>
+        <v>188</v>
+      </c>
+      <c r="AD17" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="AE17" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="AF17" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="AG17" s="1" t="s">
+        <v>192</v>
       </c>
       <c r="AH17" s="2" t="s">
-        <v>168</v>
+        <v>193</v>
       </c>
       <c r="AI17" s="2" t="s">
-        <v>169</v>
+        <v>194</v>
+      </c>
+      <c r="AJ17" s="4" t="s">
+        <v>195</v>
+      </c>
+      <c r="AK17" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="AL17" s="4" t="s">
+        <v>197</v>
+      </c>
+      <c r="AM17" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="AN17" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="AO17" s="4" t="s">
+        <v>200</v>
       </c>
     </row>
-    <row r="18" ht="62.4" spans="1:34">
+    <row r="18" ht="62.4" spans="1:41">
       <c r="A18" s="5"/>
       <c r="B18" s="5"/>
       <c r="C18" s="6"/>
@@ -3964,56 +4556,74 @@
       <c r="J18" s="5"/>
       <c r="K18" s="5"/>
       <c r="L18" s="7" t="s">
-        <v>170</v>
+        <v>201</v>
       </c>
       <c r="M18" s="5"/>
       <c r="N18" s="7" t="s">
-        <v>171</v>
+        <v>202</v>
       </c>
       <c r="O18" s="5" t="s">
-        <v>172</v>
+        <v>203</v>
       </c>
       <c r="T18" s="1" t="s">
-        <v>173</v>
+        <v>204</v>
       </c>
       <c r="U18" s="1" t="s">
-        <v>174</v>
+        <v>205</v>
       </c>
       <c r="V18" s="1" t="s">
-        <v>175</v>
+        <v>206</v>
       </c>
       <c r="X18" s="1" t="s">
-        <v>176</v>
+        <v>207</v>
       </c>
       <c r="Y18" s="1" t="s">
-        <v>177</v>
+        <v>208</v>
       </c>
       <c r="Z18" s="1" t="s">
-        <v>178</v>
+        <v>209</v>
       </c>
       <c r="AA18" s="1" t="s">
-        <v>179</v>
+        <v>210</v>
       </c>
       <c r="AB18" s="1" t="s">
-        <v>180</v>
+        <v>211</v>
       </c>
       <c r="AC18" s="1" t="s">
-        <v>181</v>
-      </c>
-      <c r="AD18" s="4" t="s">
-        <v>182</v>
-      </c>
-      <c r="AE18" s="4" t="s">
-        <v>183</v>
-      </c>
-      <c r="AF18" s="4" t="s">
-        <v>184</v>
+        <v>212</v>
+      </c>
+      <c r="AD18" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="AE18" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="AF18" s="1" t="s">
+        <v>215</v>
       </c>
       <c r="AH18" s="2" t="s">
-        <v>185</v>
+        <v>216</v>
+      </c>
+      <c r="AJ18" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="AK18" s="4" t="s">
+        <v>218</v>
+      </c>
+      <c r="AL18" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="AM18" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="AN18" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="AO18" s="4" t="s">
+        <v>222</v>
       </c>
     </row>
-    <row r="19" ht="46.8" spans="1:35">
+    <row r="19" ht="78" spans="1:41">
       <c r="A19" s="5"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
@@ -4026,355 +4636,481 @@
       <c r="J19" s="5"/>
       <c r="K19" s="5"/>
       <c r="L19" s="7" t="s">
-        <v>186</v>
+        <v>223</v>
       </c>
       <c r="M19" s="5" t="s">
-        <v>187</v>
+        <v>224</v>
       </c>
       <c r="N19" s="7" t="s">
-        <v>188</v>
+        <v>225</v>
       </c>
       <c r="O19" s="5" t="s">
-        <v>189</v>
+        <v>226</v>
       </c>
       <c r="T19" s="1" t="s">
-        <v>190</v>
+        <v>227</v>
       </c>
       <c r="U19" s="1" t="s">
-        <v>191</v>
+        <v>228</v>
       </c>
       <c r="V19" s="1" t="s">
-        <v>192</v>
+        <v>229</v>
       </c>
       <c r="Z19" s="1" t="s">
-        <v>193</v>
+        <v>230</v>
       </c>
       <c r="AA19" s="1" t="s">
-        <v>194</v>
+        <v>231</v>
       </c>
       <c r="AB19" s="1" t="s">
-        <v>195</v>
+        <v>232</v>
       </c>
       <c r="AC19" s="1" t="s">
-        <v>196</v>
-      </c>
-      <c r="AD19" s="4" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF19" s="4" t="s">
-        <v>198</v>
-      </c>
-      <c r="AG19" s="4" t="s">
-        <v>199</v>
+        <v>233</v>
+      </c>
+      <c r="AD19" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="AF19" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="AG19" s="1" t="s">
+        <v>236</v>
       </c>
       <c r="AH19" s="2" t="s">
-        <v>200</v>
+        <v>237</v>
       </c>
       <c r="AI19" s="2" t="s">
-        <v>201</v>
+        <v>238</v>
+      </c>
+      <c r="AL19" s="4" t="s">
+        <v>239</v>
+      </c>
+      <c r="AN19" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="AO19" s="4" t="s">
+        <v>241</v>
       </c>
     </row>
-    <row r="20" ht="62.4" spans="14:35">
+    <row r="20" ht="140.4" spans="14:41">
       <c r="N20" s="1" t="s">
-        <v>202</v>
+        <v>242</v>
       </c>
       <c r="O20" s="1" t="s">
-        <v>203</v>
+        <v>243</v>
       </c>
       <c r="T20" s="1" t="s">
-        <v>204</v>
+        <v>244</v>
       </c>
       <c r="V20" s="1" t="s">
-        <v>205</v>
+        <v>245</v>
       </c>
       <c r="Z20" s="1" t="s">
-        <v>206</v>
+        <v>246</v>
       </c>
       <c r="AA20" s="1" t="s">
-        <v>207</v>
+        <v>247</v>
       </c>
       <c r="AB20" s="1" t="s">
-        <v>208</v>
+        <v>248</v>
       </c>
       <c r="AH20" s="2" t="s">
-        <v>209</v>
+        <v>249</v>
       </c>
       <c r="AI20" s="2" t="s">
-        <v>210</v>
+        <v>250</v>
+      </c>
+      <c r="AL20" s="4" t="s">
+        <v>251</v>
+      </c>
+      <c r="AM20" s="4" t="s">
+        <v>252</v>
+      </c>
+      <c r="AN20" s="4" t="s">
+        <v>253</v>
+      </c>
+      <c r="AO20" s="4" t="s">
+        <v>254</v>
       </c>
     </row>
-    <row r="21" ht="46.8" spans="14:29">
+    <row r="21" ht="93.6" spans="14:41">
       <c r="N21" s="1" t="s">
-        <v>211</v>
+        <v>255</v>
       </c>
       <c r="T21" s="1" t="s">
-        <v>212</v>
+        <v>256</v>
       </c>
       <c r="U21" s="1" t="s">
-        <v>213</v>
+        <v>257</v>
       </c>
       <c r="Z21" s="1" t="s">
-        <v>214</v>
+        <v>258</v>
       </c>
       <c r="AA21" s="1" t="s">
-        <v>215</v>
+        <v>259</v>
       </c>
       <c r="AB21" s="1" t="s">
-        <v>216</v>
+        <v>260</v>
       </c>
       <c r="AC21" s="1" t="s">
-        <v>217</v>
+        <v>261</v>
+      </c>
+      <c r="AL21" s="4" t="s">
+        <v>262</v>
+      </c>
+      <c r="AN21" s="4" t="s">
+        <v>263</v>
+      </c>
+      <c r="AO21" s="4" t="s">
+        <v>264</v>
       </c>
     </row>
-    <row r="22" ht="63.6" spans="14:29">
+    <row r="22" ht="78" spans="14:41">
       <c r="N22" s="15" t="s">
-        <v>218</v>
+        <v>265</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>219</v>
+        <v>266</v>
       </c>
       <c r="T22" s="1" t="s">
-        <v>220</v>
+        <v>267</v>
       </c>
       <c r="U22" s="1" t="s">
-        <v>221</v>
+        <v>268</v>
       </c>
       <c r="Z22" s="1" t="s">
-        <v>222</v>
+        <v>269</v>
       </c>
       <c r="AA22" s="1" t="s">
-        <v>223</v>
+        <v>270</v>
       </c>
       <c r="AB22" s="1" t="s">
-        <v>224</v>
+        <v>271</v>
       </c>
       <c r="AC22" s="1" t="s">
-        <v>225</v>
+        <v>272</v>
+      </c>
+      <c r="AL22" s="4" t="s">
+        <v>273</v>
+      </c>
+      <c r="AN22" s="4" t="s">
+        <v>274</v>
+      </c>
+      <c r="AO22" s="4" t="s">
+        <v>275</v>
       </c>
     </row>
-    <row r="23" ht="31.2" spans="14:29">
+    <row r="23" ht="31.2" spans="14:41">
       <c r="N23" s="1" t="s">
-        <v>226</v>
+        <v>276</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>227</v>
+        <v>277</v>
       </c>
       <c r="Z23" s="1" t="s">
-        <v>228</v>
+        <v>278</v>
       </c>
       <c r="AA23" s="1" t="s">
-        <v>229</v>
+        <v>279</v>
       </c>
       <c r="AB23" s="1" t="s">
-        <v>230</v>
+        <v>280</v>
       </c>
       <c r="AC23" s="1" t="s">
-        <v>231</v>
+        <v>281</v>
+      </c>
+      <c r="AL23" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="AM23" s="4" t="s">
+        <v>283</v>
+      </c>
+      <c r="AN23" s="4" t="s">
+        <v>284</v>
+      </c>
+      <c r="AO23" s="4" t="s">
+        <v>285</v>
       </c>
     </row>
-    <row r="24" ht="31.2" spans="14:26">
+    <row r="24" ht="31.2" spans="14:41">
       <c r="N24" s="1" t="s">
-        <v>232</v>
+        <v>286</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>233</v>
+        <v>287</v>
       </c>
       <c r="Z24" s="1" t="s">
-        <v>234</v>
+        <v>288</v>
+      </c>
+      <c r="AL24" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="AM24" s="4" t="s">
+        <v>290</v>
+      </c>
+      <c r="AN24" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="AO24" s="4" t="s">
+        <v>292</v>
       </c>
     </row>
-    <row r="25" spans="14:27">
+    <row r="25" spans="14:41">
       <c r="N25" s="1" t="s">
-        <v>235</v>
+        <v>293</v>
       </c>
       <c r="Z25" s="1" t="s">
-        <v>236</v>
+        <v>294</v>
       </c>
       <c r="AA25" s="1" t="s">
-        <v>237</v>
+        <v>295</v>
+      </c>
+      <c r="AN25" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="AO25" s="4" t="s">
+        <v>297</v>
       </c>
     </row>
-    <row r="26" ht="46.8" spans="14:26">
+    <row r="26" ht="46.8" spans="14:41">
       <c r="N26" s="1" t="s">
-        <v>238</v>
+        <v>298</v>
       </c>
       <c r="O26" s="2" t="s">
-        <v>239</v>
+        <v>299</v>
       </c>
       <c r="Z26" s="1" t="s">
-        <v>240</v>
+        <v>300</v>
+      </c>
+      <c r="AN26" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="AO26" s="4" t="s">
+        <v>302</v>
       </c>
     </row>
-    <row r="27" spans="14:27">
+    <row r="27" spans="14:41">
       <c r="N27" s="1" t="s">
-        <v>241</v>
+        <v>303</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>242</v>
+        <v>304</v>
       </c>
       <c r="Z27" s="1" t="s">
-        <v>243</v>
+        <v>305</v>
       </c>
       <c r="AA27" s="1" t="s">
-        <v>244</v>
+        <v>306</v>
+      </c>
+      <c r="AN27" s="4" t="s">
+        <v>307</v>
+      </c>
+      <c r="AO27" s="4" t="s">
+        <v>308</v>
       </c>
     </row>
-    <row r="28" spans="14:27">
+    <row r="28" spans="14:41">
       <c r="N28" s="1" t="s">
-        <v>245</v>
+        <v>309</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>246</v>
+        <v>310</v>
       </c>
       <c r="Z28" s="1" t="s">
-        <v>247</v>
+        <v>311</v>
       </c>
       <c r="AA28" s="1" t="s">
-        <v>248</v>
+        <v>312</v>
+      </c>
+      <c r="AN28" s="4" t="s">
+        <v>313</v>
+      </c>
+      <c r="AO28" s="4" t="s">
+        <v>314</v>
       </c>
     </row>
-    <row r="29" ht="78.6" spans="14:15">
+    <row r="29" ht="78.6" spans="14:41">
       <c r="N29" s="1" t="s">
-        <v>249</v>
+        <v>315</v>
       </c>
       <c r="O29" s="1" t="s">
-        <v>250</v>
+        <v>316</v>
+      </c>
+      <c r="AN29" s="4" t="s">
+        <v>317</v>
+      </c>
+      <c r="AO29" s="4" t="s">
+        <v>318</v>
       </c>
     </row>
-    <row r="30" spans="14:15">
+    <row r="30" spans="14:41">
       <c r="N30" s="1" t="s">
-        <v>251</v>
+        <v>319</v>
       </c>
       <c r="O30" s="2" t="s">
-        <v>252</v>
+        <v>320</v>
+      </c>
+      <c r="AN30" s="4" t="s">
+        <v>321</v>
+      </c>
+      <c r="AO30" s="4" t="s">
+        <v>322</v>
       </c>
     </row>
-    <row r="31" spans="14:15">
+    <row r="31" spans="14:41">
       <c r="N31" s="1" t="s">
-        <v>253</v>
+        <v>323</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>254</v>
+        <v>324</v>
+      </c>
+      <c r="AN31" s="4" t="s">
+        <v>325</v>
+      </c>
+      <c r="AO31" s="4" t="s">
+        <v>326</v>
       </c>
     </row>
-    <row r="32" spans="14:15">
+    <row r="32" ht="31.2" spans="14:41">
       <c r="N32" s="2" t="s">
-        <v>255</v>
+        <v>327</v>
       </c>
       <c r="O32" s="2" t="s">
-        <v>256</v>
+        <v>328</v>
+      </c>
+      <c r="AN32" s="4" t="s">
+        <v>329</v>
+      </c>
+      <c r="AO32" s="4" t="s">
+        <v>330</v>
       </c>
     </row>
-    <row r="33" spans="14:15">
+    <row r="33" spans="14:41">
       <c r="N33" s="1" t="s">
-        <v>257</v>
+        <v>331</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>258</v>
+        <v>332</v>
+      </c>
+      <c r="AN33" s="4" t="s">
+        <v>333</v>
+      </c>
+      <c r="AO33" s="4" t="s">
+        <v>334</v>
       </c>
     </row>
-    <row r="34" spans="14:15">
+    <row r="34" ht="31.2" spans="14:40">
       <c r="N34" s="1" t="s">
-        <v>259</v>
+        <v>335</v>
       </c>
       <c r="O34" s="2" t="s">
-        <v>260</v>
+        <v>336</v>
+      </c>
+      <c r="AN34" s="4" t="s">
+        <v>337</v>
       </c>
     </row>
-    <row r="35" spans="14:15">
+    <row r="35" ht="78" spans="14:41">
       <c r="N35" s="1" t="s">
-        <v>261</v>
+        <v>338</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>262</v>
+        <v>339</v>
+      </c>
+      <c r="AN35" s="4" t="s">
+        <v>340</v>
+      </c>
+      <c r="AO35" s="4" t="s">
+        <v>341</v>
       </c>
     </row>
     <row r="36" spans="14:15">
       <c r="N36" s="1" t="s">
-        <v>263</v>
+        <v>342</v>
       </c>
       <c r="O36" s="2" t="s">
-        <v>264</v>
+        <v>343</v>
       </c>
     </row>
     <row r="37" spans="14:15">
       <c r="N37" s="1" t="s">
-        <v>265</v>
+        <v>344</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>266</v>
+        <v>345</v>
       </c>
     </row>
     <row r="38" spans="14:15">
       <c r="N38" s="1" t="s">
-        <v>267</v>
+        <v>346</v>
       </c>
       <c r="O38" s="2" t="s">
-        <v>268</v>
+        <v>347</v>
       </c>
     </row>
     <row r="39" spans="14:15">
       <c r="N39" s="1" t="s">
-        <v>269</v>
+        <v>348</v>
       </c>
       <c r="O39" s="2" t="s">
-        <v>270</v>
+        <v>349</v>
       </c>
     </row>
     <row r="40" spans="14:15">
       <c r="N40" s="2" t="s">
-        <v>271</v>
+        <v>350</v>
       </c>
       <c r="O40" s="2" t="s">
-        <v>272</v>
+        <v>351</v>
       </c>
     </row>
     <row r="41" spans="14:15">
       <c r="N41" s="1" t="s">
-        <v>273</v>
+        <v>352</v>
       </c>
       <c r="O41" s="2" t="s">
-        <v>274</v>
+        <v>353</v>
       </c>
     </row>
     <row r="42" spans="14:15">
       <c r="N42" s="1" t="s">
-        <v>275</v>
+        <v>354</v>
       </c>
       <c r="O42" s="2" t="s">
-        <v>276</v>
+        <v>355</v>
       </c>
     </row>
     <row r="43" spans="14:15">
       <c r="N43" s="1" t="s">
-        <v>277</v>
+        <v>356</v>
       </c>
       <c r="O43" s="2" t="s">
-        <v>278</v>
+        <v>357</v>
       </c>
     </row>
     <row r="44" spans="14:15">
       <c r="N44" s="2" t="s">
-        <v>279</v>
+        <v>358</v>
       </c>
       <c r="O44" s="2" t="s">
-        <v>280</v>
+        <v>359</v>
       </c>
     </row>
     <row r="45" spans="14:15">
       <c r="N45" s="1" t="s">
-        <v>281</v>
+        <v>360</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>282</v>
+        <v>361</v>
       </c>
     </row>
     <row r="46" ht="46.8" spans="14:15">
       <c r="N46" s="1" t="s">
-        <v>283</v>
+        <v>362</v>
       </c>
       <c r="O46" s="1" t="s">
-        <v>284</v>
+        <v>363</v>
       </c>
     </row>
   </sheetData>

</xml_diff>